<commit_message>
Changed visualizer so that abstract states are labelled with their constituent ground states in hopes that this will help debug poor abstract policy performance.
</commit_message>
<xml_diff>
--- a/Data for Michael.xlsx
+++ b/Data for Michael.xlsx
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>